<commit_message>
Archiving/Unarchiving by Year: added an archiveGroup in GroupController.java and added a findByYear function in GroupRepository.java
</commit_message>
<xml_diff>
--- a/WebBasedEvaluations/Old Program documents/Evaluation Template 001.xlsx
+++ b/WebBasedEvaluations/Old Program documents/Evaluation Template 001.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\git\Fall-2022-Group-3-Web-Evaluation\WebBasedEvaluations\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jack\cpsc488\Spring-2024-Evaluation-System-\WebBasedEvaluations\Old Program documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DE149A-7388-4463-AA30-2370611A48A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D0569B-C176-4604-9573-B55BD3138DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3FAD3DD6-7A1D-42CB-BC54-8CFE443C5D15}"/>
+    <workbookView xWindow="3585" yWindow="2745" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{3FAD3DD6-7A1D-42CB-BC54-8CFE443C5D15}"/>
   </bookViews>
   <sheets>
     <sheet name="Eval_format" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="260">
   <si>
     <t>SECTION</t>
   </si>
@@ -4873,7 +4873,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A17"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4887,11 +4887,6 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>36</v>
-      </c>
-    </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>253</v>

</xml_diff>